<commit_message>
Correction of the first test case
</commit_message>
<xml_diff>
--- a/Cases.xlsx
+++ b/Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\welcome\Desktop\fmh_android_10_11_24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D53377-59AE-4D02-9A8B-8215E1EB083A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1C957D-15B2-4727-8349-3CA7F21D1397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Тест-кейс" sheetId="1" r:id="rId1"/>
@@ -1087,9 +1087,6 @@
     <t>Ссылка на вложение (Attachments)</t>
   </si>
   <si>
-    <t>высокий</t>
-  </si>
-  <si>
     <t>Значительная(Major)</t>
   </si>
   <si>
@@ -1156,7 +1153,10 @@
     <t>Открытие по ссылке "Политика конфиденциальности" приложения "Вхосписе" не происходит</t>
   </si>
   <si>
-    <t>Открытие по ссылке "Ползовательское соглашение" приложения "Вхосписе" не происходит</t>
+    <t>10. Создание новости не удалось. (Выбрана неверная категория)</t>
+  </si>
+  <si>
+    <t>Открытие по ссылке "Пользовательское соглашение" приложения "Вхосписе" не происходит</t>
   </si>
 </sst>
 </file>
@@ -1864,7 +1864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C8" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
@@ -2600,7 +2600,7 @@
         <v>9</v>
       </c>
       <c r="B40" s="41" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C40" s="43" t="s">
         <v>314</v>
@@ -2660,13 +2660,13 @@
       <c r="D43" s="46"/>
       <c r="E43" s="44"/>
       <c r="F43" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="G43" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="G43" s="4" t="s">
-        <v>362</v>
-      </c>
       <c r="H43" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -2711,10 +2711,10 @@
         <v>25</v>
       </c>
       <c r="G46" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="H46" s="14" t="s">
         <v>363</v>
-      </c>
-      <c r="H46" s="14" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -6187,6 +6187,7 @@
     <mergeCell ref="C47:C53"/>
     <mergeCell ref="D47:D53"/>
     <mergeCell ref="E47:E53"/>
+    <mergeCell ref="A89:A98"/>
     <mergeCell ref="A239:A243"/>
     <mergeCell ref="B239:B243"/>
     <mergeCell ref="C239:C243"/>
@@ -6197,7 +6198,6 @@
     <mergeCell ref="C235:C238"/>
     <mergeCell ref="D235:D238"/>
     <mergeCell ref="E235:E238"/>
-    <mergeCell ref="A89:A98"/>
     <mergeCell ref="B89:B98"/>
     <mergeCell ref="C89:C98"/>
     <mergeCell ref="D89:D98"/>
@@ -6221,6 +6221,7 @@
     <mergeCell ref="C139:C148"/>
     <mergeCell ref="E149:E158"/>
     <mergeCell ref="C184:C194"/>
+    <mergeCell ref="B139:B148"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="C5:C7"/>
@@ -6231,7 +6232,6 @@
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="E2:E4"/>
-    <mergeCell ref="B139:B148"/>
     <mergeCell ref="D139:D148"/>
     <mergeCell ref="E139:E148"/>
     <mergeCell ref="A149:A158"/>
@@ -6354,8 +6354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{335038E4-C21C-43BC-BC07-2591900D80EC}">
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="C166" sqref="C166:C168"/>
+    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
+      <selection activeCell="C169" sqref="C169:C179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6431,10 +6431,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="41" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C3" s="45" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D3" s="43" t="s">
         <v>314</v>
@@ -6492,10 +6492,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="41" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C6" s="45" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D6" s="52" t="s">
         <v>314</v>
@@ -6553,10 +6553,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="41" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C9" s="45" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D9" s="43" t="s">
         <v>314</v>
@@ -6682,10 +6682,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="41" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C16" s="45" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D16" s="43" t="s">
         <v>314</v>
@@ -6802,7 +6802,7 @@
         <v>206</v>
       </c>
       <c r="H22" s="32" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I22" s="38"/>
     </row>
@@ -6814,7 +6814,7 @@
         <v>210</v>
       </c>
       <c r="C23" s="45" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D23" s="43" t="s">
         <v>314</v>
@@ -6931,7 +6931,7 @@
         <v>217</v>
       </c>
       <c r="H29" s="32" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I29" s="38"/>
     </row>
@@ -6940,10 +6940,10 @@
         <v>6</v>
       </c>
       <c r="B30" s="41" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C30" s="45" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D30" s="43" t="s">
         <v>314</v>
@@ -7003,13 +7003,13 @@
       <c r="D33" s="44"/>
       <c r="E33" s="44"/>
       <c r="F33" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="G33" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="G33" s="4" t="s">
-        <v>362</v>
-      </c>
       <c r="H33" s="33" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I33" s="38"/>
     </row>
@@ -7057,10 +7057,10 @@
         <v>25</v>
       </c>
       <c r="G36" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="H36" s="32" t="s">
         <v>363</v>
-      </c>
-      <c r="H36" s="32" t="s">
-        <v>364</v>
       </c>
       <c r="I36" s="38"/>
     </row>
@@ -7069,10 +7069,10 @@
         <v>7</v>
       </c>
       <c r="B37" s="41" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C37" s="45" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D37" s="43" t="s">
         <v>314</v>
@@ -7186,10 +7186,10 @@
         <v>25</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H43" s="32" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I43" s="38"/>
     </row>
@@ -7198,10 +7198,10 @@
         <v>8</v>
       </c>
       <c r="B44" s="41" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C44" s="45" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D44" s="43" t="s">
         <v>314</v>
@@ -7318,7 +7318,7 @@
         <v>234</v>
       </c>
       <c r="H50" s="32" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="I50" s="38"/>
     </row>
@@ -7327,10 +7327,10 @@
         <v>9</v>
       </c>
       <c r="B51" s="41" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C51" s="45" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D51" s="43" t="s">
         <v>314</v>
@@ -7456,10 +7456,10 @@
         <v>10</v>
       </c>
       <c r="B58" s="41" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C58" s="45" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D58" s="43" t="s">
         <v>314</v>
@@ -7588,7 +7588,7 @@
         <v>56</v>
       </c>
       <c r="C65" s="45" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D65" s="43" t="s">
         <v>314</v>
@@ -7768,7 +7768,7 @@
         <v>94</v>
       </c>
       <c r="C75" s="45" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D75" s="43" t="s">
         <v>314</v>
@@ -7948,7 +7948,7 @@
         <v>98</v>
       </c>
       <c r="C85" s="45" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D85" s="43" t="s">
         <v>314</v>
@@ -8128,7 +8128,7 @@
         <v>108</v>
       </c>
       <c r="C95" s="45" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D95" s="43" t="s">
         <v>314</v>
@@ -8308,7 +8308,7 @@
         <v>59</v>
       </c>
       <c r="C105" s="45" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D105" s="43" t="s">
         <v>314</v>
@@ -8473,7 +8473,7 @@
         <v>41</v>
       </c>
       <c r="G114" s="7" t="s">
-        <v>68</v>
+        <v>372</v>
       </c>
       <c r="H114" s="34" t="s">
         <v>69</v>
@@ -8488,7 +8488,7 @@
         <v>185</v>
       </c>
       <c r="C115" s="64" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D115" s="43" t="s">
         <v>314</v>
@@ -8668,7 +8668,7 @@
         <v>208</v>
       </c>
       <c r="C125" s="45" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D125" s="43" t="s">
         <v>314</v>
@@ -9028,7 +9028,7 @@
         <v>264</v>
       </c>
       <c r="C145" s="45" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D145" s="44" t="s">
         <v>314</v>
@@ -9225,7 +9225,7 @@
         <v>290</v>
       </c>
       <c r="C156" s="45" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D156" s="43" t="s">
         <v>314</v>
@@ -9351,10 +9351,10 @@
         <v>21</v>
       </c>
       <c r="B163" s="41" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C163" s="45" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D163" s="52" t="s">
         <v>314</v>
@@ -9415,7 +9415,7 @@
         <v>373</v>
       </c>
       <c r="C166" s="45" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D166" s="41" t="s">
         <v>314</v>
@@ -9476,7 +9476,7 @@
         <v>130</v>
       </c>
       <c r="C169" s="45" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D169" s="43" t="s">
         <v>314</v>
@@ -9673,7 +9673,7 @@
         <v>147</v>
       </c>
       <c r="C180" s="45" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D180" s="60" t="s">
         <v>314</v>
@@ -9717,7 +9717,7 @@
         <v>148</v>
       </c>
       <c r="C182" s="45" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D182" s="43" t="s">
         <v>314</v>
@@ -9795,7 +9795,7 @@
         <v>153</v>
       </c>
       <c r="C186" s="45" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D186" s="43" t="s">
         <v>314</v>
@@ -9873,7 +9873,7 @@
         <v>248</v>
       </c>
       <c r="C190" s="45" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D190" s="63" t="s">
         <v>314</v>

</xml_diff>